<commit_message>
Adding sets and data cleaning.
</commit_message>
<xml_diff>
--- a/TrainAllocation1/Railway services-2024.xlsx
+++ b/TrainAllocation1/Railway services-2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rickw\Documents\Erasmus\TA\Case Studies 2024\CaseStudies2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gebruiker/Documents/GitHub/BaWeCO1/TrainAllocation1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3BD0CF7-FEAC-4176-98AB-9E88EFF0F788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04398D4D-624F-4043-9165-21BF5C3D6FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="861" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="15840" tabRatio="861" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -202,7 +202,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Standaard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -507,22 +507,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L204"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="A177" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F206" sqref="F206"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -548,7 +548,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -578,7 +578,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="5"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -606,7 +606,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="4"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -634,7 +634,7 @@
       <c r="I4" s="1"/>
       <c r="J4" s="4"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -662,7 +662,7 @@
       <c r="I5" s="1"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -690,7 +690,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="4"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -718,7 +718,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -746,7 +746,7 @@
       <c r="I8" s="1"/>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -774,7 +774,7 @@
       <c r="I9" s="1"/>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -802,7 +802,7 @@
       <c r="I10" s="1"/>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -830,7 +830,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="4"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -858,7 +858,7 @@
       <c r="I12" s="1"/>
       <c r="J12" s="4"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -886,7 +886,7 @@
       <c r="I13" s="1"/>
       <c r="J13" s="4"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -914,7 +914,7 @@
       <c r="I14" s="1"/>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -942,7 +942,7 @@
       <c r="I15" s="1"/>
       <c r="J15" s="4"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -970,7 +970,7 @@
       <c r="I16" s="1"/>
       <c r="J16" s="4"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -998,7 +998,7 @@
       <c r="I17" s="1"/>
       <c r="J17" s="4"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1026,7 +1026,7 @@
       <c r="I18" s="1"/>
       <c r="J18" s="4"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1054,7 +1054,7 @@
       <c r="I19" s="1"/>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1082,7 +1082,7 @@
       <c r="I20" s="1"/>
       <c r="J20" s="4"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1110,7 +1110,7 @@
       <c r="I21" s="1"/>
       <c r="J21" s="4"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1138,7 +1138,7 @@
       <c r="I22" s="1"/>
       <c r="J22" s="4"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1166,7 +1166,7 @@
       <c r="I23" s="1"/>
       <c r="J23" s="4"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1194,7 +1194,7 @@
       <c r="I24" s="1"/>
       <c r="J24" s="4"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1222,7 +1222,7 @@
       <c r="I25" s="1"/>
       <c r="J25" s="4"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1250,7 +1250,7 @@
       <c r="I26" s="1"/>
       <c r="J26" s="4"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1278,7 +1278,7 @@
       <c r="I27" s="1"/>
       <c r="J27" s="4"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1306,7 +1306,7 @@
       <c r="I28" s="1"/>
       <c r="J28" s="4"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1334,7 +1334,7 @@
       <c r="I29" s="1"/>
       <c r="J29" s="4"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1362,7 +1362,7 @@
       <c r="I30" s="1"/>
       <c r="J30" s="4"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1390,7 +1390,7 @@
       <c r="I31" s="1"/>
       <c r="J31" s="4"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1418,7 +1418,7 @@
       <c r="I32" s="1"/>
       <c r="J32" s="4"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1446,7 +1446,7 @@
       <c r="I33" s="1"/>
       <c r="J33" s="4"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -1474,7 +1474,7 @@
       <c r="I34" s="1"/>
       <c r="J34" s="4"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -1502,7 +1502,7 @@
       <c r="I35" s="1"/>
       <c r="J35" s="4"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -1530,7 +1530,7 @@
       <c r="I36" s="1"/>
       <c r="J36" s="4"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -1558,7 +1558,7 @@
       <c r="I37" s="1"/>
       <c r="J37" s="4"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -1586,7 +1586,7 @@
       <c r="I38" s="1"/>
       <c r="J38" s="4"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -1614,7 +1614,7 @@
       <c r="I39" s="1"/>
       <c r="J39" s="4"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -1642,7 +1642,7 @@
       <c r="I40" s="1"/>
       <c r="J40" s="4"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -1670,7 +1670,7 @@
       <c r="I41" s="1"/>
       <c r="J41" s="4"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -1698,7 +1698,7 @@
       <c r="I42" s="1"/>
       <c r="J42" s="4"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -1726,7 +1726,7 @@
       <c r="I43" s="1"/>
       <c r="J43" s="4"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -1754,7 +1754,7 @@
       <c r="I44" s="1"/>
       <c r="J44" s="4"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -1782,7 +1782,7 @@
       <c r="I45" s="1"/>
       <c r="J45" s="4"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -1810,7 +1810,7 @@
       <c r="I46" s="1"/>
       <c r="J46" s="4"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -1838,7 +1838,7 @@
       <c r="I47" s="1"/>
       <c r="J47" s="4"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -1866,7 +1866,7 @@
       <c r="I48" s="1"/>
       <c r="J48" s="4"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -1894,7 +1894,7 @@
       <c r="I49" s="1"/>
       <c r="J49" s="4"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -1922,7 +1922,7 @@
       <c r="I50" s="1"/>
       <c r="J50" s="4"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -1950,7 +1950,7 @@
       <c r="I51" s="1"/>
       <c r="J51" s="4"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -1978,7 +1978,7 @@
       <c r="I52" s="1"/>
       <c r="J52" s="4"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -2006,7 +2006,7 @@
       <c r="I53" s="1"/>
       <c r="J53" s="4"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -2034,7 +2034,7 @@
       <c r="I54" s="1"/>
       <c r="J54" s="4"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -2062,7 +2062,7 @@
       <c r="I55" s="1"/>
       <c r="J55" s="4"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -2090,7 +2090,7 @@
       <c r="I56" s="1"/>
       <c r="J56" s="4"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -2118,7 +2118,7 @@
       <c r="I57" s="1"/>
       <c r="J57" s="4"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -2146,7 +2146,7 @@
       <c r="I58" s="1"/>
       <c r="J58" s="4"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -2174,7 +2174,7 @@
       <c r="I59" s="1"/>
       <c r="J59" s="4"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -2202,7 +2202,7 @@
       <c r="I60" s="1"/>
       <c r="J60" s="4"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -2230,7 +2230,7 @@
       <c r="I61" s="1"/>
       <c r="J61" s="4"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -2258,7 +2258,7 @@
       <c r="I62" s="1"/>
       <c r="J62" s="4"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -2286,7 +2286,7 @@
       <c r="I63" s="1"/>
       <c r="J63" s="4"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -2314,7 +2314,7 @@
       <c r="I64" s="1"/>
       <c r="J64" s="4"/>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -2342,7 +2342,7 @@
       <c r="I65" s="1"/>
       <c r="J65" s="4"/>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -2370,7 +2370,7 @@
       <c r="I66" s="1"/>
       <c r="J66" s="4"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -2398,7 +2398,7 @@
       <c r="I67" s="1"/>
       <c r="J67" s="4"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -2426,7 +2426,7 @@
       <c r="I68" s="1"/>
       <c r="J68" s="4"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -2454,7 +2454,7 @@
       <c r="I69" s="1"/>
       <c r="J69" s="4"/>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -2482,7 +2482,7 @@
       <c r="I70" s="1"/>
       <c r="J70" s="4"/>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>70</v>
       </c>
@@ -2510,7 +2510,7 @@
       <c r="I71" s="1"/>
       <c r="J71" s="4"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>71</v>
       </c>
@@ -2538,7 +2538,7 @@
       <c r="I72" s="1"/>
       <c r="J72" s="4"/>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>72</v>
       </c>
@@ -2566,7 +2566,7 @@
       <c r="I73" s="1"/>
       <c r="J73" s="4"/>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>73</v>
       </c>
@@ -2594,7 +2594,7 @@
       <c r="I74" s="1"/>
       <c r="J74" s="4"/>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>74</v>
       </c>
@@ -2622,7 +2622,7 @@
       <c r="I75" s="1"/>
       <c r="J75" s="4"/>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>75</v>
       </c>
@@ -2650,7 +2650,7 @@
       <c r="I76" s="1"/>
       <c r="J76" s="4"/>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
         <v>76</v>
       </c>
@@ -2678,7 +2678,7 @@
       <c r="I77" s="1"/>
       <c r="J77" s="4"/>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>77</v>
       </c>
@@ -2706,7 +2706,7 @@
       <c r="I78" s="1"/>
       <c r="J78" s="4"/>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>78</v>
       </c>
@@ -2734,7 +2734,7 @@
       <c r="I79" s="1"/>
       <c r="J79" s="4"/>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>79</v>
       </c>
@@ -2762,7 +2762,7 @@
       <c r="I80" s="1"/>
       <c r="J80" s="4"/>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>80</v>
       </c>
@@ -2790,7 +2790,7 @@
       <c r="I81" s="1"/>
       <c r="J81" s="4"/>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>81</v>
       </c>
@@ -2818,7 +2818,7 @@
       <c r="I82" s="1"/>
       <c r="J82" s="4"/>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>82</v>
       </c>
@@ -2846,7 +2846,7 @@
       <c r="I83" s="1"/>
       <c r="J83" s="4"/>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>83</v>
       </c>
@@ -2874,7 +2874,7 @@
       <c r="I84" s="1"/>
       <c r="J84" s="4"/>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
         <v>84</v>
       </c>
@@ -2902,7 +2902,7 @@
       <c r="I85" s="1"/>
       <c r="J85" s="4"/>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
         <v>85</v>
       </c>
@@ -2930,7 +2930,7 @@
       <c r="I86" s="1"/>
       <c r="J86" s="4"/>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
         <v>86</v>
       </c>
@@ -2958,7 +2958,7 @@
       <c r="I87" s="1"/>
       <c r="J87" s="4"/>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>87</v>
       </c>
@@ -2986,7 +2986,7 @@
       <c r="I88" s="1"/>
       <c r="J88" s="4"/>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
         <v>88</v>
       </c>
@@ -3014,7 +3014,7 @@
       <c r="I89" s="1"/>
       <c r="J89" s="4"/>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>89</v>
       </c>
@@ -3042,7 +3042,7 @@
       <c r="I90" s="1"/>
       <c r="J90" s="4"/>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
         <v>90</v>
       </c>
@@ -3070,7 +3070,7 @@
       <c r="I91" s="1"/>
       <c r="J91" s="4"/>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>91</v>
       </c>
@@ -3098,7 +3098,7 @@
       <c r="I92" s="1"/>
       <c r="J92" s="4"/>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
         <v>92</v>
       </c>
@@ -3126,7 +3126,7 @@
       <c r="I93" s="1"/>
       <c r="J93" s="4"/>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
         <v>93</v>
       </c>
@@ -3154,7 +3154,7 @@
       <c r="I94" s="1"/>
       <c r="J94" s="4"/>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
         <v>94</v>
       </c>
@@ -3182,7 +3182,7 @@
       <c r="I95" s="1"/>
       <c r="J95" s="4"/>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
         <v>95</v>
       </c>
@@ -3210,7 +3210,7 @@
       <c r="I96" s="1"/>
       <c r="J96" s="4"/>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
         <v>96</v>
       </c>
@@ -3238,7 +3238,7 @@
       <c r="I97" s="1"/>
       <c r="J97" s="4"/>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
         <v>97</v>
       </c>
@@ -3266,7 +3266,7 @@
       <c r="I98" s="1"/>
       <c r="J98" s="4"/>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
         <v>98</v>
       </c>
@@ -3294,7 +3294,7 @@
       <c r="I99" s="1"/>
       <c r="J99" s="4"/>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
         <v>99</v>
       </c>
@@ -3322,7 +3322,7 @@
       <c r="I100" s="1"/>
       <c r="J100" s="4"/>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
         <v>100</v>
       </c>
@@ -3350,7 +3350,7 @@
       <c r="I101" s="1"/>
       <c r="J101" s="4"/>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
         <v>101</v>
       </c>
@@ -3378,7 +3378,7 @@
       <c r="I102" s="1"/>
       <c r="J102" s="4"/>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
         <v>102</v>
       </c>
@@ -3406,7 +3406,7 @@
       <c r="I103" s="1"/>
       <c r="J103" s="4"/>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
         <v>103</v>
       </c>
@@ -3434,7 +3434,7 @@
       <c r="I104" s="1"/>
       <c r="J104" s="4"/>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
         <v>104</v>
       </c>
@@ -3462,7 +3462,7 @@
       <c r="I105" s="1"/>
       <c r="J105" s="4"/>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
         <v>105</v>
       </c>
@@ -3490,7 +3490,7 @@
       <c r="I106" s="1"/>
       <c r="J106" s="4"/>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
         <v>106</v>
       </c>
@@ -3518,7 +3518,7 @@
       <c r="I107" s="1"/>
       <c r="J107" s="4"/>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
         <v>107</v>
       </c>
@@ -3546,7 +3546,7 @@
       <c r="I108" s="1"/>
       <c r="J108" s="4"/>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
         <v>108</v>
       </c>
@@ -3574,7 +3574,7 @@
       <c r="I109" s="1"/>
       <c r="J109" s="4"/>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
         <v>109</v>
       </c>
@@ -3602,7 +3602,7 @@
       <c r="I110" s="1"/>
       <c r="J110" s="4"/>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
         <v>110</v>
       </c>
@@ -3630,7 +3630,7 @@
       <c r="I111" s="1"/>
       <c r="J111" s="4"/>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
         <v>111</v>
       </c>
@@ -3658,7 +3658,7 @@
       <c r="I112" s="1"/>
       <c r="J112" s="4"/>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A113" s="2">
         <v>112</v>
       </c>
@@ -3686,7 +3686,7 @@
       <c r="I113" s="1"/>
       <c r="J113" s="4"/>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
         <v>113</v>
       </c>
@@ -3714,7 +3714,7 @@
       <c r="I114" s="1"/>
       <c r="J114" s="4"/>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
         <v>114</v>
       </c>
@@ -3742,7 +3742,7 @@
       <c r="I115" s="1"/>
       <c r="J115" s="4"/>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
         <v>115</v>
       </c>
@@ -3770,7 +3770,7 @@
       <c r="I116" s="1"/>
       <c r="J116" s="4"/>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A117" s="2">
         <v>116</v>
       </c>
@@ -3798,7 +3798,7 @@
       <c r="I117" s="1"/>
       <c r="J117" s="4"/>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
         <v>117</v>
       </c>
@@ -3826,7 +3826,7 @@
       <c r="I118" s="1"/>
       <c r="J118" s="4"/>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
         <v>118</v>
       </c>
@@ -3854,7 +3854,7 @@
       <c r="I119" s="1"/>
       <c r="J119" s="4"/>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
         <v>119</v>
       </c>
@@ -3882,7 +3882,7 @@
       <c r="I120" s="1"/>
       <c r="J120" s="4"/>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
         <v>120</v>
       </c>
@@ -3910,7 +3910,7 @@
       <c r="I121" s="1"/>
       <c r="J121" s="4"/>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
         <v>121</v>
       </c>
@@ -3938,7 +3938,7 @@
       <c r="I122" s="1"/>
       <c r="J122" s="4"/>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A123" s="2">
         <v>122</v>
       </c>
@@ -3966,7 +3966,7 @@
       <c r="I123" s="1"/>
       <c r="J123" s="4"/>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A124" s="2">
         <v>123</v>
       </c>
@@ -3994,7 +3994,7 @@
       <c r="I124" s="1"/>
       <c r="J124" s="4"/>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A125" s="2">
         <v>124</v>
       </c>
@@ -4022,7 +4022,7 @@
       <c r="I125" s="1"/>
       <c r="J125" s="4"/>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A126" s="2">
         <v>125</v>
       </c>
@@ -4050,7 +4050,7 @@
       <c r="I126" s="1"/>
       <c r="J126" s="4"/>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A127" s="2">
         <v>126</v>
       </c>
@@ -4078,7 +4078,7 @@
       <c r="I127" s="1"/>
       <c r="J127" s="4"/>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A128" s="2">
         <v>127</v>
       </c>
@@ -4106,7 +4106,7 @@
       <c r="I128" s="1"/>
       <c r="J128" s="4"/>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A129" s="2">
         <v>128</v>
       </c>
@@ -4134,7 +4134,7 @@
       <c r="I129" s="1"/>
       <c r="J129" s="4"/>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A130" s="2">
         <v>129</v>
       </c>
@@ -4162,7 +4162,7 @@
       <c r="I130" s="1"/>
       <c r="J130" s="4"/>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A131" s="2">
         <v>130</v>
       </c>
@@ -4190,7 +4190,7 @@
       <c r="I131" s="1"/>
       <c r="J131" s="4"/>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A132" s="2">
         <v>131</v>
       </c>
@@ -4218,7 +4218,7 @@
       <c r="I132" s="1"/>
       <c r="J132" s="4"/>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A133" s="2">
         <v>132</v>
       </c>
@@ -4246,7 +4246,7 @@
       <c r="I133" s="1"/>
       <c r="J133" s="4"/>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A134" s="2">
         <v>133</v>
       </c>
@@ -4274,7 +4274,7 @@
       <c r="I134" s="1"/>
       <c r="J134" s="4"/>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A135" s="2">
         <v>134</v>
       </c>
@@ -4302,7 +4302,7 @@
       <c r="I135" s="1"/>
       <c r="J135" s="4"/>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A136" s="2">
         <v>135</v>
       </c>
@@ -4330,7 +4330,7 @@
       <c r="I136" s="1"/>
       <c r="J136" s="4"/>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A137" s="2">
         <v>136</v>
       </c>
@@ -4358,7 +4358,7 @@
       <c r="I137" s="1"/>
       <c r="J137" s="4"/>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A138" s="2">
         <v>137</v>
       </c>
@@ -4386,7 +4386,7 @@
       <c r="I138" s="1"/>
       <c r="J138" s="4"/>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A139" s="2">
         <v>138</v>
       </c>
@@ -4414,7 +4414,7 @@
       <c r="I139" s="1"/>
       <c r="J139" s="4"/>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A140" s="2">
         <v>139</v>
       </c>
@@ -4442,7 +4442,7 @@
       <c r="I140" s="1"/>
       <c r="J140" s="4"/>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A141" s="2">
         <v>140</v>
       </c>
@@ -4470,7 +4470,7 @@
       <c r="I141" s="1"/>
       <c r="J141" s="4"/>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A142" s="2">
         <v>141</v>
       </c>
@@ -4498,7 +4498,7 @@
       <c r="I142" s="1"/>
       <c r="J142" s="4"/>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A143" s="2">
         <v>142</v>
       </c>
@@ -4526,7 +4526,7 @@
       <c r="I143" s="1"/>
       <c r="J143" s="4"/>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A144" s="2">
         <v>143</v>
       </c>
@@ -4554,7 +4554,7 @@
       <c r="I144" s="1"/>
       <c r="J144" s="4"/>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A145" s="2">
         <v>144</v>
       </c>
@@ -4582,7 +4582,7 @@
       <c r="I145" s="1"/>
       <c r="J145" s="4"/>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A146" s="2">
         <v>145</v>
       </c>
@@ -4610,7 +4610,7 @@
       <c r="I146" s="1"/>
       <c r="J146" s="4"/>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A147" s="2">
         <v>146</v>
       </c>
@@ -4638,7 +4638,7 @@
       <c r="I147" s="1"/>
       <c r="J147" s="4"/>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A148" s="2">
         <v>147</v>
       </c>
@@ -4666,7 +4666,7 @@
       <c r="I148" s="1"/>
       <c r="J148" s="4"/>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A149" s="2">
         <v>148</v>
       </c>
@@ -4694,7 +4694,7 @@
       <c r="I149" s="1"/>
       <c r="J149" s="4"/>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A150" s="2">
         <v>149</v>
       </c>
@@ -4722,7 +4722,7 @@
       <c r="I150" s="1"/>
       <c r="J150" s="4"/>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A151" s="2">
         <v>150</v>
       </c>
@@ -4750,7 +4750,7 @@
       <c r="I151" s="1"/>
       <c r="J151" s="4"/>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A152" s="2">
         <v>151</v>
       </c>
@@ -4778,7 +4778,7 @@
       <c r="I152" s="1"/>
       <c r="J152" s="4"/>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A153" s="2">
         <v>152</v>
       </c>
@@ -4806,7 +4806,7 @@
       <c r="I153" s="1"/>
       <c r="J153" s="4"/>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A154" s="2">
         <v>153</v>
       </c>
@@ -4834,7 +4834,7 @@
       <c r="I154" s="1"/>
       <c r="J154" s="4"/>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A155" s="2">
         <v>154</v>
       </c>
@@ -4862,7 +4862,7 @@
       <c r="I155" s="1"/>
       <c r="J155" s="4"/>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A156" s="2">
         <v>155</v>
       </c>
@@ -4890,7 +4890,7 @@
       <c r="I156" s="1"/>
       <c r="J156" s="4"/>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A157" s="2">
         <v>156</v>
       </c>
@@ -4918,7 +4918,7 @@
       <c r="I157" s="1"/>
       <c r="J157" s="4"/>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A158" s="2">
         <v>157</v>
       </c>
@@ -4946,7 +4946,7 @@
       <c r="I158" s="1"/>
       <c r="J158" s="4"/>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A159" s="2">
         <v>158</v>
       </c>
@@ -4974,7 +4974,7 @@
       <c r="I159" s="1"/>
       <c r="J159" s="4"/>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A160" s="2">
         <v>159</v>
       </c>
@@ -5002,7 +5002,7 @@
       <c r="I160" s="1"/>
       <c r="J160" s="4"/>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A161" s="2">
         <v>160</v>
       </c>
@@ -5030,7 +5030,7 @@
       <c r="I161" s="1"/>
       <c r="J161" s="4"/>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A162" s="2">
         <v>161</v>
       </c>
@@ -5058,7 +5058,7 @@
       <c r="I162" s="1"/>
       <c r="J162" s="4"/>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A163" s="2">
         <v>162</v>
       </c>
@@ -5086,7 +5086,7 @@
       <c r="I163" s="1"/>
       <c r="J163" s="4"/>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A164" s="2">
         <v>163</v>
       </c>
@@ -5114,7 +5114,7 @@
       <c r="I164" s="1"/>
       <c r="J164" s="4"/>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A165" s="2">
         <v>164</v>
       </c>
@@ -5142,7 +5142,7 @@
       <c r="I165" s="1"/>
       <c r="J165" s="4"/>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A166" s="2">
         <v>165</v>
       </c>
@@ -5170,7 +5170,7 @@
       <c r="I166" s="1"/>
       <c r="J166" s="4"/>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A167" s="2">
         <v>166</v>
       </c>
@@ -5198,7 +5198,7 @@
       <c r="I167" s="1"/>
       <c r="J167" s="4"/>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A168" s="2">
         <v>167</v>
       </c>
@@ -5226,7 +5226,7 @@
       <c r="I168" s="1"/>
       <c r="J168" s="4"/>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A169" s="2">
         <v>168</v>
       </c>
@@ -5254,7 +5254,7 @@
       <c r="I169" s="1"/>
       <c r="J169" s="4"/>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A170" s="2">
         <v>169</v>
       </c>
@@ -5282,7 +5282,7 @@
       <c r="I170" s="1"/>
       <c r="J170" s="4"/>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A171" s="2">
         <v>170</v>
       </c>
@@ -5310,7 +5310,7 @@
       <c r="I171" s="1"/>
       <c r="J171" s="4"/>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A172" s="2">
         <v>171</v>
       </c>
@@ -5338,7 +5338,7 @@
       <c r="I172" s="1"/>
       <c r="J172" s="4"/>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A173" s="2">
         <v>172</v>
       </c>
@@ -5366,7 +5366,7 @@
       <c r="I173" s="1"/>
       <c r="J173" s="4"/>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A174" s="2">
         <v>173</v>
       </c>
@@ -5394,7 +5394,7 @@
       <c r="I174" s="1"/>
       <c r="J174" s="4"/>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A175" s="2">
         <v>174</v>
       </c>
@@ -5422,7 +5422,7 @@
       <c r="I175" s="1"/>
       <c r="J175" s="4"/>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A176" s="2">
         <v>175</v>
       </c>
@@ -5450,7 +5450,7 @@
       <c r="I176" s="1"/>
       <c r="J176" s="4"/>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A177" s="2">
         <v>176</v>
       </c>
@@ -5478,7 +5478,7 @@
       <c r="I177" s="1"/>
       <c r="J177" s="4"/>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A178" s="2">
         <v>177</v>
       </c>
@@ -5506,7 +5506,7 @@
       <c r="I178" s="1"/>
       <c r="J178" s="4"/>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A179" s="2">
         <v>178</v>
       </c>
@@ -5534,7 +5534,7 @@
       <c r="I179" s="1"/>
       <c r="J179" s="4"/>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A180" s="2">
         <v>179</v>
       </c>
@@ -5562,7 +5562,7 @@
       <c r="I180" s="1"/>
       <c r="J180" s="4"/>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A181" s="2">
         <v>180</v>
       </c>
@@ -5590,7 +5590,7 @@
       <c r="I181" s="1"/>
       <c r="J181" s="4"/>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A182" s="2">
         <v>181</v>
       </c>
@@ -5618,7 +5618,7 @@
       <c r="I182" s="1"/>
       <c r="J182" s="4"/>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A183" s="2">
         <v>182</v>
       </c>
@@ -5646,7 +5646,7 @@
       <c r="I183" s="1"/>
       <c r="J183" s="4"/>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A184" s="2">
         <v>183</v>
       </c>
@@ -5674,7 +5674,7 @@
       <c r="I184" s="1"/>
       <c r="J184" s="4"/>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A185" s="2">
         <v>184</v>
       </c>
@@ -5702,7 +5702,7 @@
       <c r="I185" s="1"/>
       <c r="J185" s="4"/>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A186" s="2">
         <v>185</v>
       </c>
@@ -5730,7 +5730,7 @@
       <c r="I186" s="1"/>
       <c r="J186" s="4"/>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A187" s="2">
         <v>186</v>
       </c>
@@ -5758,7 +5758,7 @@
       <c r="I187" s="1"/>
       <c r="J187" s="4"/>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A188" s="2">
         <v>187</v>
       </c>
@@ -5786,7 +5786,7 @@
       <c r="I188" s="1"/>
       <c r="J188" s="4"/>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A189" s="2">
         <v>188</v>
       </c>
@@ -5814,7 +5814,7 @@
       <c r="I189" s="1"/>
       <c r="J189" s="4"/>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A190" s="2">
         <v>189</v>
       </c>
@@ -5842,7 +5842,7 @@
       <c r="I190" s="1"/>
       <c r="J190" s="4"/>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A191" s="2">
         <v>190</v>
       </c>
@@ -5870,7 +5870,7 @@
       <c r="I191" s="1"/>
       <c r="J191" s="4"/>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A192" s="2">
         <v>191</v>
       </c>
@@ -5898,7 +5898,7 @@
       <c r="I192" s="1"/>
       <c r="J192" s="4"/>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A193" s="2">
         <v>192</v>
       </c>
@@ -5926,7 +5926,7 @@
       <c r="I193" s="1"/>
       <c r="J193" s="4"/>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A194" s="2">
         <v>193</v>
       </c>
@@ -5954,7 +5954,7 @@
       <c r="I194" s="1"/>
       <c r="J194" s="4"/>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A195" s="2">
         <v>194</v>
       </c>
@@ -5982,7 +5982,7 @@
       <c r="I195" s="1"/>
       <c r="J195" s="4"/>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A196" s="2">
         <v>195</v>
       </c>
@@ -6010,7 +6010,7 @@
       <c r="I196" s="1"/>
       <c r="J196" s="4"/>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A197" s="2">
         <v>196</v>
       </c>
@@ -6038,7 +6038,7 @@
       <c r="I197" s="1"/>
       <c r="J197" s="4"/>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A198" s="2">
         <v>197</v>
       </c>
@@ -6066,7 +6066,7 @@
       <c r="I198" s="1"/>
       <c r="J198" s="4"/>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A199" s="2">
         <v>198</v>
       </c>
@@ -6094,7 +6094,7 @@
       <c r="I199" s="1"/>
       <c r="J199" s="4"/>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A200" s="2">
         <v>199</v>
       </c>
@@ -6122,7 +6122,7 @@
       <c r="I200" s="1"/>
       <c r="J200" s="4"/>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A201" s="2">
         <v>200</v>
       </c>
@@ -6150,17 +6150,11 @@
       <c r="I201" s="1"/>
       <c r="J201" s="4"/>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F203" s="4">
-        <f>COUNTIF(F2:F201,"&gt;1400")</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F204" s="4">
-        <f>MAX(F2:F201)</f>
-        <v>1497</v>
-      </c>
+    <row r="203" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F203" s="4"/>
+    </row>
+    <row r="204" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F204" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6174,7 +6168,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>